<commit_message>
correction export de candidatures
</commit_message>
<xml_diff>
--- a/src/main/resources/template/candidatures_template.xlsx
+++ b/src/main/resources/template/candidatures_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="2445" windowWidth="18555" windowHeight="5610"/>
   </bookViews>
   <sheets>
-    <sheet name="${codCommission}" sheetId="1" r:id="rId1"/>
+    <sheet name="${code}" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -705,7 +705,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Correction bug dans certains établissements sur l'autosizing de colonnes
</commit_message>
<xml_diff>
--- a/src/main/resources/template/candidatures_template.xlsx
+++ b/src/main/resources/template/candidatures_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18555" windowHeight="5610"/>
+    <workbookView xWindow="2640" yWindow="705" windowWidth="18555" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="${code}" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>&lt;jt:hideCols test="${etablissementHide}"&gt;Dernier établissement&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:hideCols test="${lastDipHide}"&gt;Dernier diplome&lt;/jt:hideCols&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:hideCols test="${libFormHide}"&gt;Libellé formation&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>${footer}</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${lastDipHide}"&gt;Dernier diplôme&lt;/jt:hideCols&gt;</t>
   </si>
 </sst>
 </file>
@@ -702,10 +702,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -715,18 +715,30 @@
     <col min="3" max="3" width="18.140625" style="4" customWidth="1"/>
     <col min="4" max="5" width="24.5703125" style="4" customWidth="1"/>
     <col min="6" max="10" width="19.5703125" style="4" customWidth="1"/>
-    <col min="11" max="24" width="15.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23" style="4" customWidth="1"/>
+    <col min="13" max="21" width="15.5703125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="27.85546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="26.140625" style="4" customWidth="1"/>
     <col min="25" max="25" width="16.140625" style="4" customWidth="1"/>
     <col min="26" max="26" width="25.140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="4" customWidth="1"/>
-    <col min="28" max="33" width="13.7109375" style="4" customWidth="1"/>
-    <col min="34" max="34" width="16.28515625" style="4" customWidth="1"/>
-    <col min="35" max="37" width="12.85546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" style="4" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1"/>
+    <col min="29" max="29" width="21" style="4" customWidth="1"/>
+    <col min="30" max="30" width="45" style="4" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="22" style="4" customWidth="1"/>
+    <col min="33" max="33" width="24.140625" style="4" customWidth="1"/>
+    <col min="34" max="34" width="22.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="27.85546875" style="4" customWidth="1"/>
+    <col min="36" max="36" width="48.28515625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="14.5703125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="19.7109375" style="4" customWidth="1"/>
+    <col min="39" max="39" width="15.42578125" style="4" customWidth="1"/>
     <col min="40" max="46" width="22" style="4" customWidth="1"/>
-    <col min="47" max="47" width="7" style="4" customWidth="1"/>
-    <col min="48" max="48" width="22" style="4" customWidth="1"/>
+    <col min="47" max="47" width="18.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="28.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -743,7 +755,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -752,13 +764,13 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>20</v>
@@ -773,106 +785,106 @@
         <v>23</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
@@ -889,22 +901,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>10</v>
@@ -916,37 +928,37 @@
         <v>12</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="V2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>7</v>
@@ -955,25 +967,25 @@
         <v>3</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="AH2" s="4" t="s">
         <v>5</v>
@@ -982,48 +994,48 @@
         <v>6</v>
       </c>
       <c r="AJ2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="AL2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AM2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AO2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AQ2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="AV2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>

</xml_diff>

<commit_message>
correction sur les candidatues annulées ajout de la date d'annulation dans l'export ajout des candidatures annulées dans les stats modifications sur la recherche pour les petits noms
</commit_message>
<xml_diff>
--- a/src/main/resources/template/candidatures_template.xlsx
+++ b/src/main/resources/template/candidatures_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -298,13 +298,25 @@
     <t>${cand.candidat.lastLibDiplome}</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${cand.temAcceptCand!=null}"&gt;&lt;jt:if test="${cand.temAcceptCand}" then="CONFIRMATION" else="DESISTEMENT"/&gt;&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>${footer}</t>
   </si>
   <si>
     <t>&lt;jt:hideCols test="${lastDipHide}"&gt;Dernier diplôme&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${datAnnulHide}"&gt;Date annulation&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${userAnnulHide}"&gt;Annulé par&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${cand.temAcceptCand!=null}"&gt;&lt;jt:if test="${cand.temAcceptCand}" then="CONFIRMATION" else="DESISTEMENT"/&gt;&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>${cand.userAnnulCand}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${cand.datAnnulCand!=null}"&gt;${cand.datAnnulCand}&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>
@@ -700,12 +712,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV3"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -739,9 +751,10 @@
     <col min="40" max="46" width="22" style="4" customWidth="1"/>
     <col min="47" max="47" width="18.42578125" style="4" customWidth="1"/>
     <col min="48" max="48" width="28.28515625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -809,7 +822,7 @@
         <v>24</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>91</v>
@@ -886,8 +899,14 @@
       <c r="AV1" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="AW1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1030,12 +1049,18 @@
         <v>49</v>
       </c>
       <c r="AV2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>

</xml_diff>

<commit_message>
ajout d'une date de depot de piece a positionner manuellement
</commit_message>
<xml_diff>
--- a/src/main/resources/template/candidatures_template.xlsx
+++ b/src/main/resources/template/candidatures_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Présél. Lieu&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
-    <t>${cand.lastTypeDecision.preselectDateTypeDecCand}</t>
-  </si>
-  <si>
     <t>${cand.lastTypeDecision.preselectLieuTypeDecCand}</t>
   </si>
   <si>
@@ -310,13 +307,28 @@
     <t>&lt;jt:hideCols test="${userAnnulHide}"&gt;Annulé par&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
+    <t>${cand.userAnnulCand}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${cand.datAnnulCandStr}</t>
+  </si>
+  <si>
+    <t>${cand.datNewConfirmCandStr}</t>
+  </si>
+  <si>
+    <t>${cand.datNewRetourCandStr}</t>
+  </si>
+  <si>
     <t>&lt;jt:if test="${cand.temAcceptCand!=null}"&gt;&lt;jt:if test="${cand.temAcceptCand}" then="CONFIRMATION" else="DESISTEMENT"/&gt;&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>${cand.userAnnulCand}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${cand.datAnnulCandStr}</t>
+    <t>${cand.lastTypeDecision.preselectDateTypeDecCandStr}</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${datNewConfirmHide}"&gt;Date confirm. manuelle/LC&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${datNewRetourHide}"&gt;Date retour manuelle&lt;/jt:hideCols&gt;</t>
   </si>
 </sst>
 </file>
@@ -399,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -412,6 +424,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,12 +726,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="AS13" sqref="AS13"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -751,11 +764,11 @@
     <col min="39" max="39" width="15.42578125" style="4" customWidth="1"/>
     <col min="40" max="46" width="22" style="4" customWidth="1"/>
     <col min="47" max="47" width="18.42578125" style="4" customWidth="1"/>
-    <col min="48" max="48" width="28.28515625" style="4" customWidth="1"/>
-    <col min="49" max="49" width="16.5703125" customWidth="1"/>
+    <col min="48" max="50" width="28.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -823,10 +836,10 @@
         <v>24</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>13</v>
@@ -898,16 +911,22 @@
         <v>55</v>
       </c>
       <c r="AV1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -975,10 +994,10 @@
         <v>43</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>7</v>
@@ -1038,30 +1057,36 @@
         <v>51</v>
       </c>
       <c r="AR2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT2" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="AV2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY2" t="s">
         <v>98</v>
       </c>
-      <c r="AW2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>99</v>
+      <c r="AZ2" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1110,8 +1135,10 @@
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
-      <c r="AW3" s="7"/>
-      <c r="AX3" s="7"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="6"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>